<commit_message>
Just backing up. PSDR2 is receiving well, image rejection is good. Gain pot settings work. Audio out works (to earphones only, the speaker fails pretty badly, not sure why, but that's hardware anyway)
</commit_message>
<xml_diff>
--- a/Hardware/PSDR2_BOM.xlsx
+++ b/Hardware/PSDR2_BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="296">
   <si>
     <t>SMA_BOARD_EDGE</t>
   </si>
@@ -376,9 +376,6 @@
   </si>
   <si>
     <t>U4</t>
-  </si>
-  <si>
-    <t>GP-1513</t>
   </si>
   <si>
     <t>U5</t>
@@ -922,7 +919,7 @@
     <t>Lipo</t>
   </si>
   <si>
-    <t>Check mouser or other places for expensive parts….</t>
+    <t>GP39-1513</t>
   </si>
 </sst>
 </file>
@@ -1304,10 +1301,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H92"/>
+  <dimension ref="A1:H91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1325,28 +1322,28 @@
   <sheetData>
     <row r="1" spans="1:8" ht="30">
       <c r="A1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>159</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1360,7 +1357,7 @@
         <v>53</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="30">
@@ -1374,54 +1371,54 @@
         <v>44</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30">
       <c r="A4" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B4" s="5">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>131</v>
-      </c>
       <c r="H4" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B5" s="5">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" s="5">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B6" s="5">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>152</v>
-      </c>
       <c r="H6" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B7" s="5">
         <v>2</v>
@@ -1430,26 +1427,26 @@
         <v>115</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B8" s="5">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>143</v>
-      </c>
       <c r="H8" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B9" s="5">
         <v>2</v>
@@ -1458,105 +1455,105 @@
         <v>114</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="45">
       <c r="A10" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B10" s="5">
-        <v>1</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>123</v>
-      </c>
       <c r="H10" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B11" s="5">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B11" s="5">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>146</v>
-      </c>
       <c r="H11" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12" s="5">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B12" s="5">
-        <v>1</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>125</v>
-      </c>
       <c r="H12" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B13" s="5">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B13" s="5">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>129</v>
-      </c>
       <c r="H13" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B14" s="5">
         <v>2</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B15" s="5">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B15" s="5">
-        <v>1</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>150</v>
-      </c>
       <c r="H15" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B16" s="5">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B16" s="5">
-        <v>1</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>154</v>
-      </c>
       <c r="H16" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1573,12 +1570,12 @@
         <v>8</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B18" s="5">
         <v>2</v>
@@ -1592,7 +1589,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B19" s="5">
         <v>6</v>
@@ -1604,12 +1601,12 @@
         <v>19</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B20" s="5">
         <v>2</v>
@@ -1621,12 +1618,12 @@
         <v>39</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B21" s="5">
         <v>4</v>
@@ -1638,12 +1635,12 @@
         <v>17</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B22" s="5">
         <v>4</v>
@@ -1655,12 +1652,12 @@
         <v>18</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="30">
       <c r="A23" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B23" s="5">
         <v>12</v>
@@ -1672,12 +1669,12 @@
         <v>15</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B24" s="5">
         <v>4</v>
@@ -1689,12 +1686,12 @@
         <v>16</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B25" s="5">
         <v>4</v>
@@ -1706,12 +1703,12 @@
         <v>20</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B26" s="5">
         <v>2</v>
@@ -1723,29 +1720,29 @@
         <v>35</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="45">
       <c r="A27" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B27" s="5">
         <v>17</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B28" s="5">
         <v>4</v>
@@ -1757,12 +1754,12 @@
         <v>28</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="30">
       <c r="A29" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B29" s="5">
         <v>9</v>
@@ -1774,12 +1771,12 @@
         <v>5</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B30" s="5">
         <v>2</v>
@@ -1791,12 +1788,12 @@
         <v>33</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B31" s="5">
         <v>4</v>
@@ -1808,7 +1805,7 @@
         <v>37</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1825,12 +1822,12 @@
         <v>23</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B33" s="5">
         <v>4</v>
@@ -1842,12 +1839,12 @@
         <v>10</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B34" s="5">
         <v>4</v>
@@ -1859,12 +1856,12 @@
         <v>31</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="105">
       <c r="A35" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B35" s="9">
         <v>56</v>
@@ -1876,12 +1873,12 @@
         <v>2</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="45">
       <c r="A36" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B36" s="5">
         <v>13</v>
@@ -1893,12 +1890,12 @@
         <v>12</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="45">
       <c r="A37" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B37" s="5">
         <v>14</v>
@@ -1910,12 +1907,12 @@
         <v>25</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B38" s="5">
         <v>5</v>
@@ -1927,21 +1924,21 @@
         <v>29</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B39" s="5">
+        <v>1</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B39" s="5">
-        <v>1</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>141</v>
-      </c>
       <c r="H39" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1955,21 +1952,21 @@
         <v>117</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="30">
       <c r="A41" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B41" s="5">
+        <v>1</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B41" s="5">
-        <v>1</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>127</v>
-      </c>
       <c r="H41" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1983,7 +1980,7 @@
         <v>111</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="75">
@@ -1994,10 +1991,10 @@
         <v>1</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>119</v>
+        <v>295</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -2011,7 +2008,7 @@
         <v>46</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2028,12 +2025,12 @@
         <v>55</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B46" s="5">
         <v>8</v>
@@ -2045,12 +2042,12 @@
         <v>49</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B47" s="5">
         <v>4</v>
@@ -2062,7 +2059,7 @@
         <v>48</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -2076,7 +2073,7 @@
         <v>59</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="30">
@@ -2093,35 +2090,35 @@
         <v>42</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B50" s="5">
         <v>2</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B51" s="5">
+        <v>1</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B51" s="5">
-        <v>1</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>121</v>
-      </c>
       <c r="H51" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -2135,26 +2132,26 @@
         <v>61</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B53" s="5">
+        <v>1</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B53" s="5">
-        <v>1</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="H53" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B54" s="5">
         <v>4</v>
@@ -2163,21 +2160,21 @@
         <v>62</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B55" s="5">
         <v>5</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -2193,21 +2190,21 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B57" s="5">
         <v>4</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="30">
       <c r="A58" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B58" s="5">
         <v>20</v>
@@ -2219,12 +2216,12 @@
         <v>70</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="45">
       <c r="A59" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B59" s="5">
         <v>19</v>
@@ -2236,7 +2233,7 @@
         <v>102</v>
       </c>
       <c r="H59" s="8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -2253,12 +2250,12 @@
         <v>100</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="30">
       <c r="A61" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B61" s="5">
         <v>14</v>
@@ -2270,7 +2267,7 @@
         <v>68</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="30">
@@ -2287,7 +2284,7 @@
         <v>94</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2304,12 +2301,12 @@
         <v>89</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B64" s="5">
         <v>4</v>
@@ -2321,12 +2318,12 @@
         <v>104</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B65" s="5">
         <v>2</v>
@@ -2338,7 +2335,7 @@
         <v>74</v>
       </c>
       <c r="H65" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2355,12 +2352,12 @@
         <v>86</v>
       </c>
       <c r="H66" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B67" s="5">
         <v>7</v>
@@ -2372,7 +2369,7 @@
         <v>72</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -2389,12 +2386,12 @@
         <v>97</v>
       </c>
       <c r="H68" s="4" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="30">
       <c r="A69" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B69" s="5">
         <v>8</v>
@@ -2406,12 +2403,12 @@
         <v>66</v>
       </c>
       <c r="H69" s="8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="70" spans="1:8">
       <c r="A70" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B70" s="5">
         <v>2</v>
@@ -2423,12 +2420,12 @@
         <v>106</v>
       </c>
       <c r="H70" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="71" spans="1:8">
       <c r="A71" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B71" s="5">
         <v>2</v>
@@ -2440,12 +2437,12 @@
         <v>76</v>
       </c>
       <c r="H71" s="8" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B72" s="5">
         <v>2</v>
@@ -2457,7 +2454,7 @@
         <v>81</v>
       </c>
       <c r="H72" s="8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2474,7 +2471,7 @@
         <v>79</v>
       </c>
       <c r="H73" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -2491,7 +2488,7 @@
         <v>92</v>
       </c>
       <c r="H74" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -2508,12 +2505,12 @@
         <v>109</v>
       </c>
       <c r="H75" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="76" spans="1:8">
       <c r="A76" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B76" s="5">
         <v>4</v>
@@ -2525,12 +2522,12 @@
         <v>83</v>
       </c>
       <c r="H76" s="8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="77" spans="1:8">
       <c r="A77" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B77" s="5">
         <v>2</v>
@@ -2542,29 +2539,29 @@
         <v>64</v>
       </c>
       <c r="H77" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="30">
       <c r="A78" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B78" s="5">
         <v>3</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H78" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="79" spans="1:8">
       <c r="A79" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B79" s="5">
         <v>2</v>
@@ -2573,21 +2570,21 @@
         <v>0</v>
       </c>
       <c r="H79" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="30">
       <c r="A80" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B80" s="5">
+        <v>1</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B80" s="5">
-        <v>1</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="H80" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="30">
@@ -2601,21 +2598,21 @@
         <v>113</v>
       </c>
       <c r="H81" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="82" spans="1:8">
       <c r="A82" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B82" s="5">
+        <v>1</v>
+      </c>
+      <c r="C82" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B82" s="5">
-        <v>1</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>139</v>
-      </c>
       <c r="H82" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -2635,10 +2632,10 @@
         <v>0.3</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H84" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -2646,16 +2643,16 @@
         <v>0.3</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H85" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="86" spans="1:8">
       <c r="B86" s="10"/>
       <c r="C86" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -2664,9 +2661,9 @@
     <row r="88" spans="1:8">
       <c r="B88" s="10"/>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" ht="30">
       <c r="A89" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B89" s="5">
         <f>COUNT(B2:B85)</f>
@@ -2675,7 +2672,7 @@
     </row>
     <row r="90" spans="1:8">
       <c r="A90" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B90" s="5">
         <f>SUM(B2:B85)</f>
@@ -2684,11 +2681,6 @@
     </row>
     <row r="91" spans="1:8">
       <c r="B91" s="5"/>
-    </row>
-    <row r="92" spans="1:8" ht="30">
-      <c r="C92" s="2" t="s">
-        <v>296</v>
-      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F83">

</xml_diff>

<commit_message>
Update to bring github up to date with my files.
</commit_message>
<xml_diff>
--- a/Hardware/PSDR2_BOM.xlsx
+++ b/Hardware/PSDR2_BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="14355" windowHeight="6315"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="14355" windowHeight="5505"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="310">
   <si>
     <t>SMA_BOARD_EDGE</t>
   </si>
@@ -920,6 +920,48 @@
   </si>
   <si>
     <t>GP39-1513</t>
+  </si>
+  <si>
+    <t>Amp Board</t>
+  </si>
+  <si>
+    <t>LM3410XMF/NOPBCT-ND</t>
+  </si>
+  <si>
+    <t>IC DRVR WT/OLED BCKLT SOT23-5</t>
+  </si>
+  <si>
+    <t>10uH</t>
+  </si>
+  <si>
+    <t>0805 Inductors</t>
+  </si>
+  <si>
+    <t>INDUCTOR 2.2UH 260MA 20% SMD</t>
+  </si>
+  <si>
+    <t>2.2uH</t>
+  </si>
+  <si>
+    <t>587-2043-1-ND</t>
+  </si>
+  <si>
+    <t>RES 1.74 OHM 1/10W 1% 0603 SMD</t>
+  </si>
+  <si>
+    <t>541-1.74HHCT-ND</t>
+  </si>
+  <si>
+    <t>INDUCTOR 15UH 20% 0805 SMD</t>
+  </si>
+  <si>
+    <t>587-3020-1-ND</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 40V SOD323</t>
+  </si>
+  <si>
+    <t>SD101CWSTPMSCT-ND</t>
   </si>
 </sst>
 </file>
@@ -1301,10 +1343,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H91"/>
+  <dimension ref="A1:J99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2587,7 +2629,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="30">
+    <row r="81" spans="1:10" ht="30">
       <c r="A81" s="2" t="s">
         <v>112</v>
       </c>
@@ -2601,7 +2643,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:10">
       <c r="A82" s="2" t="s">
         <v>137</v>
       </c>
@@ -2615,7 +2657,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:10">
       <c r="A83" s="2" t="s">
         <v>50</v>
       </c>
@@ -2626,7 +2668,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:10">
       <c r="A84" s="1"/>
       <c r="B84" s="5">
         <v>0.3</v>
@@ -2638,7 +2680,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:10">
       <c r="B85" s="5">
         <v>0.3</v>
       </c>
@@ -2649,38 +2691,130 @@
         <v>267</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:10">
       <c r="B86" s="10"/>
       <c r="C86" s="2" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:10">
       <c r="B87" s="10"/>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:10">
       <c r="B88" s="10"/>
     </row>
-    <row r="89" spans="1:8" ht="30">
-      <c r="A89" s="2" t="s">
+    <row r="89" spans="1:10" ht="30">
+      <c r="B89" s="10">
+        <v>1</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="H89" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="J89" s="4" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10">
+      <c r="B90" s="10">
+        <v>0</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="H90" s="4" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10">
+      <c r="B91" s="10">
+        <v>0</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H91" s="4" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10">
+      <c r="B92" s="10">
+        <v>2</v>
+      </c>
+      <c r="C92" t="s">
+        <v>301</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="H92" s="4" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" ht="30">
+      <c r="B93" s="10">
+        <v>2</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="H93" s="4" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10">
+      <c r="B94" s="10">
+        <v>1</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="H94" s="4" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
+      <c r="B95" s="10">
+        <v>1</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="H95" s="4" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10">
+      <c r="B96" s="10"/>
+    </row>
+    <row r="97" spans="1:2" ht="30">
+      <c r="A97" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="B89" s="5">
+      <c r="B97" s="5">
         <f>COUNT(B2:B85)</f>
         <v>84</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
-      <c r="A90" s="2" t="s">
+    <row r="98" spans="1:2">
+      <c r="A98" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B90" s="5">
+      <c r="B98" s="5">
         <f>SUM(B2:B85)</f>
         <v>336.6</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
-      <c r="B91" s="5"/>
+    <row r="99" spans="1:2">
+      <c r="B99" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F83">

</xml_diff>